<commit_message>
chore(backlog): update product backlog with proper points proportions
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devamin/Documents/GitHub/GroupProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{634AA69F-546E-FE4F-ACCD-0C2F1321CCF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF95D2C4-413E-0A4C-B837-6DFF55BE110C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,10 +101,12 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -213,6 +215,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -222,9 +227,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +448,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -458,24 +460,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="13">
       <c r="A3" s="1" t="s">
@@ -504,8 +506,8 @@
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9">
-        <v>8</v>
+      <c r="C4" s="4">
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
@@ -524,7 +526,7 @@
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="4">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -544,7 +546,7 @@
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="4">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -564,8 +566,8 @@
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9">
-        <v>9</v>
+      <c r="C7" s="4">
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
@@ -584,8 +586,8 @@
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9">
-        <v>5</v>
+      <c r="C8" s="4">
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
@@ -604,8 +606,8 @@
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="9">
-        <v>12</v>
+      <c r="C9" s="4">
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -624,8 +626,8 @@
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="9">
-        <v>6</v>
+      <c r="C10" s="4">
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
@@ -644,8 +646,8 @@
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="9">
-        <v>4</v>
+      <c r="C11" s="4">
+        <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>

</xml_diff>